<commit_message>
Update SAP sales invoice generation process
</commit_message>
<xml_diff>
--- a/resources/VendasSAP.xlsx
+++ b/resources/VendasSAP.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A155"/>
+  <dimension ref="A1:A152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,771 +368,756 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5100234186</v>
+        <v>5100234227</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5100234219</v>
+        <v>5100234253</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5100234236</v>
+        <v>5100234176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5100234227</v>
+        <v>5100234201</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5100234253</v>
+        <v>5100234226</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5100234176</v>
+        <v>5100234260</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5100234201</v>
+        <v>5100234184</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5100234226</v>
+        <v>7160001534</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5100234260</v>
+        <v>5100234291</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5100234184</v>
+        <v>5100234286</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7160001534</v>
+        <v>5100234307</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5100234291</v>
+        <v>5100234335</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5100234286</v>
+        <v>7160001543</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5100234307</v>
+        <v>5100234362</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5100234335</v>
+        <v>5100234350</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7160001543</v>
+        <v>5100234353</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5100234362</v>
+        <v>5100193021</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5100234350</v>
+        <v>5100193029</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5100234353</v>
+        <v>7160001128</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5100193021</v>
+        <v>5100193085</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>5100193029</v>
+        <v>5100193084</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7160001128</v>
+        <v>5100193063</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5100193085</v>
+        <v>5100193093</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5100193084</v>
+        <v>5100193115</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5100193063</v>
+        <v>5100234208</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5100193093</v>
+        <v>5100234234</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>5100193115</v>
+        <v>5100234174</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5100234208</v>
+        <v>5100234189</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>5100234234</v>
+        <v>5100234222</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5100234174</v>
+        <v>5100234242</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>5100234189</v>
+        <v>5100234179</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>5100234222</v>
+        <v>5100234232</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>5100234242</v>
+        <v>5100234264</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>5100234179</v>
+        <v>5100234288</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>5100234232</v>
+        <v>5100234282</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>5100234264</v>
+        <v>5100234267</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>5100234288</v>
+        <v>5100234292</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>5100234282</v>
+        <v>7160001540</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>5100234267</v>
+        <v>5100234327</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>5100234292</v>
+        <v>5100234295</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>7160001540</v>
+        <v>5100234297</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>5100234327</v>
+        <v>5100234314</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5100234295</v>
+        <v>5100234317</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>5100234297</v>
+        <v>5100234304</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>5100234314</v>
+        <v>5100234332</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>5100234317</v>
+        <v>5100234342</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>5100234304</v>
+        <v>5100234365</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5100234332</v>
+        <v>5100234379</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>5100234342</v>
+        <v>5100234360</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>5100234365</v>
+        <v>5100234377</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>5100234379</v>
+        <v>5100193056</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>5100234360</v>
+        <v>5100193025</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>5100234377</v>
+        <v>7160001121</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5100193056</v>
+        <v>5100193031</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>5100193025</v>
+        <v>5100193061</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>7160001121</v>
+        <v>5100193040</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>5100193031</v>
+        <v>5100193027</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>5100193061</v>
+        <v>7160001125</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>5100193040</v>
+        <v>5100193060</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>5100193027</v>
+        <v>5100193071</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>7160001125</v>
+        <v>5100193067</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>5100193060</v>
+        <v>5100193103</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>5100193071</v>
+        <v>7160001116</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>5100193067</v>
+        <v>7160001117</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>5100193103</v>
+        <v>5100193098</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>7160001116</v>
+        <v>5100193095</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>7160001117</v>
+        <v>5100234290</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>5100193098</v>
+        <v>5100234330</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>5100193095</v>
+        <v>5100193087</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>5100234290</v>
+        <v>5100234228</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>5100234330</v>
+        <v>7160001539</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>5100193087</v>
+        <v>5100193064</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>5100234228</v>
+        <v>7160001132</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>7160001539</v>
+        <v>5100234250</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>5100193064</v>
+        <v>7160001533</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>7160001132</v>
+        <v>5100234261</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>5100234250</v>
+        <v>5100234363</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>7160001533</v>
+        <v>5100193041</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>5100234261</v>
+        <v>7160001130</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>5100234363</v>
+        <v>5100193112</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>5100193041</v>
+        <v>7160001126</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>7160001130</v>
+        <v>7160001118</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>5100193112</v>
+        <v>5100234266</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>7160001126</v>
+        <v>5100234289</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>7160001118</v>
+        <v>5100234331</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>5100234266</v>
+        <v>7160001123</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>5100234289</v>
+        <v>5100234318</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>5100234331</v>
+        <v>5100234339</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>7160001123</v>
+        <v>5100234346</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>5100234318</v>
+        <v>5100193062</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>5100234339</v>
+        <v>5100234341</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5100234346</v>
+        <v>5100234354</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>5100193062</v>
+        <v>7160001119</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>5100234341</v>
+        <v>5100234209</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>5100234354</v>
+        <v>5100234265</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>7160001119</v>
+        <v>5100234333</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>5100234209</v>
+        <v>5100234357</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>5100234265</v>
+        <v>7160001122</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>5100234333</v>
+        <v>5100193116</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>5100234357</v>
+        <v>5100234311</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>7160001122</v>
+        <v>5100234378</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>5100193116</v>
+        <v>5100193058</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>5100234311</v>
+        <v>5100193037</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>5100234378</v>
+        <v>5100193100</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>5100193058</v>
+        <v>5100234206</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>5100193037</v>
+        <v>5100234182</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>5100193100</v>
+        <v>7160001112</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>5100234206</v>
+        <v>5100234229</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>5100234182</v>
+        <v>5100234248</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>7160001112</v>
+        <v>5100234241</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>5100234229</v>
+        <v>5100234280</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>5100234248</v>
+        <v>5100234312</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>5100234241</v>
+        <v>5100234326</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>5100234280</v>
+        <v>5100193034</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>5100234312</v>
+        <v>5100193070</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>5100234326</v>
+        <v>7160001113</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>5100193034</v>
+        <v>5100193096</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>5100193070</v>
+        <v>5100234180</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>7160001113</v>
+        <v>5100234212</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>5100193096</v>
+        <v>5100234233</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>5100234180</v>
+        <v>5100234268</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>5100234212</v>
+        <v>5100234338</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>5100234233</v>
+        <v>5100234349</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>5100234268</v>
+        <v>5100193046</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>5100234338</v>
+        <v>5100193081</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>5100234349</v>
+        <v>7160001114</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>5100193046</v>
+        <v>7160001115</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>5100193081</v>
+        <v>5100234237</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>7160001114</v>
+        <v>5100234188</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>7160001115</v>
+        <v>5100234281</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>5100234237</v>
+        <v>5100193054</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>5100234188</v>
+        <v>5100193051</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>5100234281</v>
+        <v>5100193066</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>5100193054</v>
+        <v>5100193088</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>5100193051</v>
+        <v>5100193101</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>5100193066</v>
+        <v>5100234220</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>5100193088</v>
+        <v>5100234238</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>5100193101</v>
+        <v>5100234278</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>5100234220</v>
+        <v>5100234293</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>5100234238</v>
+        <v>5100234358</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>5100234278</v>
+        <v>5100234372</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>5100234293</v>
+        <v>5100234373</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>5100234358</v>
+        <v>5100193065</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>5100234372</v>
+        <v>5100193105</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>5100234373</v>
+        <v>5100234175</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>5100193065</v>
+        <v>5100234194</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>5100193105</v>
+        <v>5100234221</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>5100234175</v>
+        <v>5100234240</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>5100234194</v>
+        <v>5100234294</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>5100234221</v>
+        <v>5100234300</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>5100234240</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>5100234294</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>5100234300</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155">
         <v>5100193072</v>
       </c>
     </row>

</xml_diff>